<commit_message>
correction calcul desag sur Z et Y
</commit_message>
<xml_diff>
--- a/data/agg_matrix_opti_S.xlsx
+++ b/data/agg_matrix_opti_S.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubuntu\M2_EEET\Modelisation_Prospective\Projet_modelisation\MatMat-Trade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869685A6-FF9E-4B29-B40D-8FA8816A9755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1EB684-BF7C-45BA-A120-EFA7E3E7C152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8628" yWindow="2304" windowWidth="11664" windowHeight="8964" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sector_ref" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="128">
   <si>
     <t>category</t>
   </si>
@@ -409,16 +409,19 @@
     <t>Brazil, Mexico</t>
   </si>
   <si>
-    <t>China, Middle East</t>
-  </si>
-  <si>
     <t>Asia, Row Europe</t>
   </si>
   <si>
-    <t>RoW America,Turkey, Australia, Taïwan</t>
+    <t>Japan, Indonesia, RoW Africa</t>
   </si>
   <si>
-    <t>Japan, Indonesia, RoW Africa</t>
+    <t>China, RoW Asia and Pacific</t>
+  </si>
+  <si>
+    <t>RoW America,Turkey, Taïwan</t>
+  </si>
+  <si>
+    <t>RoW Middle East, Australia</t>
   </si>
 </sst>
 </file>
@@ -14446,7 +14449,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
@@ -14486,16 +14489,16 @@
         <v>50</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>122</v>
@@ -14504,7 +14507,7 @@
         <v>65</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M1" s="27" t="s">
         <v>120</v>
@@ -16050,10 +16053,10 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -16334,13 +16337,13 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -16498,13 +16501,13 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50">
         <v>0</v>

</xml_diff>